<commit_message>
Updated CIPM Level 2 Volume 1
</commit_message>
<xml_diff>
--- a/CIPM/Level 2 Volume 1.xlsx
+++ b/CIPM/Level 2 Volume 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kc111\Dev\CIPM\CIPM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1C179D-5680-43A0-B54D-8008D6A2DB22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF2C0E2-542E-4FFF-B38A-0B8C03DC8CE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="1" xr2:uid="{A0219E52-BC5C-483A-9CFD-680264FDC4D2}"/>
+    <workbookView xWindow="5700" yWindow="2292" windowWidth="24540" windowHeight="13176" xr2:uid="{A0219E52-BC5C-483A-9CFD-680264FDC4D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Performance Measurement" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -989,9 +989,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1001,23 +998,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="10" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1358,7 +1358,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{888B23C4-E01B-4DB3-AB70-0D12783B2017}">
   <dimension ref="A3:BC20"/>
   <sheetViews>
-    <sheetView topLeftCell="AL1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="BD6" sqref="BD6"/>
     </sheetView>
   </sheetViews>
@@ -2761,7 +2761,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAB0978-76AD-4949-969A-8C69EDDE888F}">
   <dimension ref="A1:BV21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AZ13" sqref="AZ13"/>
     </sheetView>
   </sheetViews>
@@ -2838,14 +2838,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:74" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="106" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="107"/>
-      <c r="F1" s="107"/>
+      <c r="B1" s="106"/>
+      <c r="C1" s="106"/>
+      <c r="D1" s="106"/>
+      <c r="E1" s="106"/>
+      <c r="F1" s="106"/>
       <c r="BH1" s="22"/>
       <c r="BI1" s="22"/>
       <c r="BJ1" s="22"/>
@@ -2969,25 +2969,25 @@
         <v>127</v>
       </c>
       <c r="AX4" s="103"/>
-      <c r="AY4" s="105" t="s">
+      <c r="AY4" s="104" t="s">
         <v>120</v>
       </c>
-      <c r="AZ4" s="105" t="s">
+      <c r="AZ4" s="104" t="s">
         <v>121</v>
       </c>
-      <c r="BH4" s="104" t="s">
+      <c r="BH4" s="107" t="s">
         <v>9</v>
       </c>
-      <c r="BI4" s="104"/>
-      <c r="BJ4" s="104" t="s">
+      <c r="BI4" s="107"/>
+      <c r="BJ4" s="107" t="s">
         <v>127</v>
       </c>
-      <c r="BK4" s="104"/>
-      <c r="BL4" s="104" t="s">
+      <c r="BK4" s="107"/>
+      <c r="BL4" s="107" t="s">
         <v>128</v>
       </c>
-      <c r="BM4" s="104"/>
-      <c r="BN4" s="105" t="s">
+      <c r="BM4" s="107"/>
+      <c r="BN4" s="104" t="s">
         <v>121</v>
       </c>
       <c r="BO4" s="71" t="s">
@@ -3119,8 +3119,8 @@
       <c r="AX5" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="AY5" s="106"/>
-      <c r="AZ5" s="106"/>
+      <c r="AY5" s="105"/>
+      <c r="AZ5" s="105"/>
       <c r="BC5" s="54" t="s">
         <v>107</v>
       </c>
@@ -3148,7 +3148,7 @@
       <c r="BM5" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="BN5" s="106"/>
+      <c r="BN5" s="105"/>
       <c r="BO5" s="71" t="s">
         <v>144</v>
       </c>
@@ -4200,11 +4200,16 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="AW13:AX13"/>
-    <mergeCell ref="P3:U3"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AW4:AX4"/>
-    <mergeCell ref="AY4:AY5"/>
+    <mergeCell ref="BG3:BM3"/>
+    <mergeCell ref="BH4:BI4"/>
+    <mergeCell ref="BJ4:BK4"/>
+    <mergeCell ref="BL4:BM4"/>
+    <mergeCell ref="BN4:BN5"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="I3:N3"/>
     <mergeCell ref="AZ4:AZ5"/>
     <mergeCell ref="AT3:AZ3"/>
     <mergeCell ref="X3:AC3"/>
@@ -4214,16 +4219,11 @@
     <mergeCell ref="AM3:AR3"/>
     <mergeCell ref="AM4:AN4"/>
     <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="I3:N3"/>
-    <mergeCell ref="BG3:BM3"/>
-    <mergeCell ref="BH4:BI4"/>
-    <mergeCell ref="BJ4:BK4"/>
-    <mergeCell ref="BL4:BM4"/>
-    <mergeCell ref="BN4:BN5"/>
+    <mergeCell ref="AW13:AX13"/>
+    <mergeCell ref="P3:U3"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AW4:AX4"/>
+    <mergeCell ref="AY4:AY5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4235,10 +4235,10 @@
   <dimension ref="A1:EK21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="DB7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="DH7" sqref="DH7"/>
+      <selection pane="bottomRight" activeCell="CI7" sqref="CI7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -4427,69 +4427,69 @@
       <c r="BO1" s="111"/>
       <c r="BP1" s="111"/>
       <c r="BQ1" s="111"/>
-      <c r="BS1" s="107" t="s">
+      <c r="BS1" s="106" t="s">
         <v>33</v>
       </c>
-      <c r="BT1" s="107"/>
-      <c r="BU1" s="107"/>
-      <c r="BV1" s="107"/>
-      <c r="BW1" s="107"/>
-      <c r="BX1" s="107"/>
-      <c r="BY1" s="107"/>
-      <c r="BZ1" s="107"/>
-      <c r="CA1" s="107"/>
-      <c r="CB1" s="107"/>
-      <c r="CC1" s="107"/>
-      <c r="CD1" s="107"/>
-      <c r="CE1" s="107"/>
-      <c r="CF1" s="107"/>
-      <c r="CG1" s="107"/>
-      <c r="CH1" s="107"/>
-      <c r="CI1" s="107"/>
-      <c r="CJ1" s="107"/>
-      <c r="CK1" s="107"/>
-      <c r="CL1" s="107"/>
-      <c r="CM1" s="107"/>
-      <c r="CN1" s="107"/>
-      <c r="CO1" s="107"/>
-      <c r="CP1" s="107"/>
-      <c r="CQ1" s="107"/>
-      <c r="CR1" s="107"/>
-      <c r="CS1" s="107"/>
-      <c r="CT1" s="107"/>
-      <c r="CU1" s="107"/>
-      <c r="CV1" s="107"/>
-      <c r="CW1" s="107"/>
-      <c r="CX1" s="107"/>
-      <c r="CY1" s="107"/>
-      <c r="CZ1" s="107"/>
-      <c r="DA1" s="107"/>
-      <c r="DC1" s="107" t="s">
+      <c r="BT1" s="106"/>
+      <c r="BU1" s="106"/>
+      <c r="BV1" s="106"/>
+      <c r="BW1" s="106"/>
+      <c r="BX1" s="106"/>
+      <c r="BY1" s="106"/>
+      <c r="BZ1" s="106"/>
+      <c r="CA1" s="106"/>
+      <c r="CB1" s="106"/>
+      <c r="CC1" s="106"/>
+      <c r="CD1" s="106"/>
+      <c r="CE1" s="106"/>
+      <c r="CF1" s="106"/>
+      <c r="CG1" s="106"/>
+      <c r="CH1" s="106"/>
+      <c r="CI1" s="106"/>
+      <c r="CJ1" s="106"/>
+      <c r="CK1" s="106"/>
+      <c r="CL1" s="106"/>
+      <c r="CM1" s="106"/>
+      <c r="CN1" s="106"/>
+      <c r="CO1" s="106"/>
+      <c r="CP1" s="106"/>
+      <c r="CQ1" s="106"/>
+      <c r="CR1" s="106"/>
+      <c r="CS1" s="106"/>
+      <c r="CT1" s="106"/>
+      <c r="CU1" s="106"/>
+      <c r="CV1" s="106"/>
+      <c r="CW1" s="106"/>
+      <c r="CX1" s="106"/>
+      <c r="CY1" s="106"/>
+      <c r="CZ1" s="106"/>
+      <c r="DA1" s="106"/>
+      <c r="DC1" s="106" t="s">
         <v>48</v>
       </c>
-      <c r="DD1" s="107"/>
-      <c r="DE1" s="107"/>
-      <c r="DF1" s="107"/>
-      <c r="DG1" s="107"/>
-      <c r="DH1" s="107"/>
-      <c r="DI1" s="107"/>
-      <c r="DJ1" s="107"/>
-      <c r="DK1" s="107"/>
-      <c r="DL1" s="107"/>
-      <c r="DM1" s="107"/>
-      <c r="DN1" s="107"/>
-      <c r="DO1" s="107"/>
-      <c r="DP1" s="107"/>
-      <c r="DQ1" s="107"/>
-      <c r="DR1" s="107"/>
-      <c r="DS1" s="107"/>
-      <c r="DT1" s="107"/>
-      <c r="DU1" s="107"/>
-      <c r="DV1" s="107"/>
-      <c r="DW1" s="107"/>
-      <c r="DX1" s="107"/>
-      <c r="DY1" s="107"/>
-      <c r="DZ1" s="107"/>
+      <c r="DD1" s="106"/>
+      <c r="DE1" s="106"/>
+      <c r="DF1" s="106"/>
+      <c r="DG1" s="106"/>
+      <c r="DH1" s="106"/>
+      <c r="DI1" s="106"/>
+      <c r="DJ1" s="106"/>
+      <c r="DK1" s="106"/>
+      <c r="DL1" s="106"/>
+      <c r="DM1" s="106"/>
+      <c r="DN1" s="106"/>
+      <c r="DO1" s="106"/>
+      <c r="DP1" s="106"/>
+      <c r="DQ1" s="106"/>
+      <c r="DR1" s="106"/>
+      <c r="DS1" s="106"/>
+      <c r="DT1" s="106"/>
+      <c r="DU1" s="106"/>
+      <c r="DV1" s="106"/>
+      <c r="DW1" s="106"/>
+      <c r="DX1" s="106"/>
+      <c r="DY1" s="106"/>
+      <c r="DZ1" s="106"/>
       <c r="EA1" s="23"/>
     </row>
     <row r="2" spans="1:141" s="16" customFormat="1" x14ac:dyDescent="0.3">
@@ -4717,15 +4717,15 @@
       <c r="DF3" s="102"/>
       <c r="DG3" s="102"/>
       <c r="DH3" s="102"/>
-      <c r="DJ3" s="108" t="s">
+      <c r="DJ3" s="113" t="s">
         <v>68</v>
       </c>
-      <c r="DK3" s="108"/>
-      <c r="DL3" s="108"/>
-      <c r="DN3" s="108" t="s">
+      <c r="DK3" s="113"/>
+      <c r="DL3" s="113"/>
+      <c r="DN3" s="113" t="s">
         <v>64</v>
       </c>
-      <c r="DO3" s="108"/>
+      <c r="DO3" s="113"/>
       <c r="DQ3" s="102" t="s">
         <v>90</v>
       </c>
@@ -4781,37 +4781,37 @@
       <c r="BG4" s="44"/>
       <c r="BH4" s="44"/>
       <c r="BW4" s="31"/>
-      <c r="DJ4" s="108"/>
-      <c r="DK4" s="108"/>
-      <c r="DL4" s="108"/>
-      <c r="DN4" s="108"/>
-      <c r="DO4" s="108"/>
+      <c r="DJ4" s="113"/>
+      <c r="DK4" s="113"/>
+      <c r="DL4" s="113"/>
+      <c r="DN4" s="113"/>
+      <c r="DO4" s="113"/>
     </row>
     <row r="5" spans="1:141" s="5" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I5" s="109">
+      <c r="I5" s="110">
         <v>41455</v>
       </c>
-      <c r="J5" s="109"/>
-      <c r="K5" s="109">
+      <c r="J5" s="110"/>
+      <c r="K5" s="110">
         <v>41639</v>
       </c>
-      <c r="L5" s="109"/>
-      <c r="M5" s="109"/>
+      <c r="L5" s="110"/>
+      <c r="M5" s="110"/>
       <c r="N5" s="103" t="s">
         <v>14</v>
       </c>
       <c r="O5" s="103"/>
       <c r="P5" s="103"/>
-      <c r="S5" s="110" t="s">
+      <c r="S5" s="112" t="s">
         <v>15</v>
       </c>
-      <c r="T5" s="110"/>
-      <c r="U5" s="110"/>
-      <c r="W5" s="110" t="s">
+      <c r="T5" s="112"/>
+      <c r="U5" s="112"/>
+      <c r="W5" s="112" t="s">
         <v>15</v>
       </c>
-      <c r="X5" s="110"/>
-      <c r="Y5" s="110"/>
+      <c r="X5" s="112"/>
+      <c r="Y5" s="112"/>
       <c r="AB5" s="103" t="s">
         <v>26</v>
       </c>
@@ -4842,50 +4842,50 @@
       <c r="AU5" s="103"/>
       <c r="AV5" s="103"/>
       <c r="AW5" s="103"/>
-      <c r="AY5" s="105" t="s">
+      <c r="AY5" s="104" t="s">
         <v>78</v>
       </c>
-      <c r="AZ5" s="105" t="s">
+      <c r="AZ5" s="104" t="s">
         <v>63</v>
       </c>
-      <c r="BA5" s="104" t="s">
+      <c r="BA5" s="107" t="s">
         <v>9</v>
       </c>
-      <c r="BB5" s="104"/>
-      <c r="BC5" s="112" t="s">
+      <c r="BB5" s="107"/>
+      <c r="BC5" s="108" t="s">
         <v>12</v>
       </c>
-      <c r="BD5" s="112"/>
-      <c r="BE5" s="113" t="s">
+      <c r="BD5" s="108"/>
+      <c r="BE5" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="BF5" s="113"/>
-      <c r="BG5" s="113" t="s">
+      <c r="BF5" s="109"/>
+      <c r="BG5" s="109" t="s">
         <v>87</v>
       </c>
-      <c r="BH5" s="113"/>
-      <c r="BJ5" s="105" t="s">
+      <c r="BH5" s="109"/>
+      <c r="BJ5" s="104" t="s">
         <v>78</v>
       </c>
-      <c r="BK5" s="105" t="s">
+      <c r="BK5" s="104" t="s">
         <v>63</v>
       </c>
-      <c r="BL5" s="105" t="s">
+      <c r="BL5" s="104" t="s">
         <v>79</v>
       </c>
-      <c r="BM5" s="105" t="s">
+      <c r="BM5" s="104" t="s">
         <v>80</v>
       </c>
-      <c r="BN5" s="105" t="s">
+      <c r="BN5" s="104" t="s">
         <v>81</v>
       </c>
-      <c r="BO5" s="105" t="s">
+      <c r="BO5" s="104" t="s">
         <v>82</v>
       </c>
-      <c r="BP5" s="105" t="s">
+      <c r="BP5" s="104" t="s">
         <v>83</v>
       </c>
-      <c r="BQ5" s="105" t="s">
+      <c r="BQ5" s="104" t="s">
         <v>8</v>
       </c>
       <c r="BU5" s="5" cm="1">
@@ -4927,12 +4927,12 @@
       <c r="CY5" s="103"/>
       <c r="CZ5" s="103"/>
       <c r="DA5" s="103"/>
-      <c r="DD5" s="109">
+      <c r="DD5" s="110">
         <v>41455</v>
       </c>
-      <c r="DE5" s="109"/>
-      <c r="DF5" s="109"/>
-      <c r="DG5" s="109"/>
+      <c r="DE5" s="110"/>
+      <c r="DF5" s="110"/>
+      <c r="DG5" s="110"/>
       <c r="DH5" s="30">
         <v>41639</v>
       </c>
@@ -5077,8 +5077,8 @@
       <c r="AW6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="AY6" s="106"/>
-      <c r="AZ6" s="106"/>
+      <c r="AY6" s="105"/>
+      <c r="AZ6" s="105"/>
       <c r="BA6" s="37" t="s">
         <v>10</v>
       </c>
@@ -5103,14 +5103,14 @@
       <c r="BH6" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="BJ6" s="106"/>
-      <c r="BK6" s="106"/>
-      <c r="BL6" s="106"/>
-      <c r="BM6" s="106"/>
-      <c r="BN6" s="106"/>
-      <c r="BO6" s="106"/>
-      <c r="BP6" s="106"/>
-      <c r="BQ6" s="106"/>
+      <c r="BJ6" s="105"/>
+      <c r="BK6" s="105"/>
+      <c r="BL6" s="105"/>
+      <c r="BM6" s="105"/>
+      <c r="BN6" s="105"/>
+      <c r="BO6" s="105"/>
+      <c r="BP6" s="105"/>
+      <c r="BQ6" s="105"/>
       <c r="BT6" s="5" t="s">
         <v>43</v>
       </c>
@@ -8617,14 +8617,40 @@
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="AZ5:AZ6"/>
-    <mergeCell ref="AA3:AM3"/>
-    <mergeCell ref="AY5:AY6"/>
-    <mergeCell ref="BY3:CE3"/>
-    <mergeCell ref="BA5:BB5"/>
-    <mergeCell ref="BC5:BD5"/>
-    <mergeCell ref="BE5:BF5"/>
-    <mergeCell ref="BZ5:CE5"/>
+    <mergeCell ref="DC1:DZ1"/>
+    <mergeCell ref="DN3:DO4"/>
+    <mergeCell ref="DJ3:DL4"/>
+    <mergeCell ref="DC3:DH3"/>
+    <mergeCell ref="CG3:CP3"/>
+    <mergeCell ref="DQ3:DZ3"/>
+    <mergeCell ref="BS1:DA1"/>
+    <mergeCell ref="BS3:BW3"/>
+    <mergeCell ref="CR3:DA3"/>
+    <mergeCell ref="K5:M5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="R4:U4"/>
+    <mergeCell ref="V4:Y4"/>
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="W5:Y5"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="AO3:AW3"/>
+    <mergeCell ref="AY1:BQ1"/>
+    <mergeCell ref="A3:P3"/>
+    <mergeCell ref="AY3:BH3"/>
+    <mergeCell ref="R3:Y3"/>
+    <mergeCell ref="AP13:AS13"/>
+    <mergeCell ref="AT13:AW13"/>
+    <mergeCell ref="AF5:AI5"/>
+    <mergeCell ref="AF13:AI13"/>
+    <mergeCell ref="AJ5:AM5"/>
+    <mergeCell ref="AJ13:AM13"/>
+    <mergeCell ref="AT5:AW5"/>
+    <mergeCell ref="AP5:AS5"/>
+    <mergeCell ref="AO11:AW11"/>
+    <mergeCell ref="AA11:AM11"/>
+    <mergeCell ref="AB13:AE13"/>
+    <mergeCell ref="AB5:AE5"/>
     <mergeCell ref="CG5:CP5"/>
     <mergeCell ref="BG5:BH5"/>
     <mergeCell ref="EC3:EK3"/>
@@ -8639,40 +8665,14 @@
     <mergeCell ref="BQ5:BQ6"/>
     <mergeCell ref="BJ3:BQ3"/>
     <mergeCell ref="CS5:DA5"/>
-    <mergeCell ref="AP13:AS13"/>
-    <mergeCell ref="AT13:AW13"/>
-    <mergeCell ref="AF5:AI5"/>
-    <mergeCell ref="AF13:AI13"/>
-    <mergeCell ref="AJ5:AM5"/>
-    <mergeCell ref="AJ13:AM13"/>
-    <mergeCell ref="AT5:AW5"/>
-    <mergeCell ref="AP5:AS5"/>
-    <mergeCell ref="AO11:AW11"/>
-    <mergeCell ref="AA11:AM11"/>
-    <mergeCell ref="AB13:AE13"/>
-    <mergeCell ref="AB5:AE5"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="AO3:AW3"/>
-    <mergeCell ref="AY1:BQ1"/>
-    <mergeCell ref="A3:P3"/>
-    <mergeCell ref="AY3:BH3"/>
-    <mergeCell ref="R3:Y3"/>
-    <mergeCell ref="K5:M5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="N5:P5"/>
-    <mergeCell ref="R4:U4"/>
-    <mergeCell ref="V4:Y4"/>
-    <mergeCell ref="S5:U5"/>
-    <mergeCell ref="W5:Y5"/>
-    <mergeCell ref="DC1:DZ1"/>
-    <mergeCell ref="DN3:DO4"/>
-    <mergeCell ref="DJ3:DL4"/>
-    <mergeCell ref="DC3:DH3"/>
-    <mergeCell ref="CG3:CP3"/>
-    <mergeCell ref="DQ3:DZ3"/>
-    <mergeCell ref="BS1:DA1"/>
-    <mergeCell ref="BS3:BW3"/>
-    <mergeCell ref="CR3:DA3"/>
+    <mergeCell ref="AZ5:AZ6"/>
+    <mergeCell ref="AA3:AM3"/>
+    <mergeCell ref="AY5:AY6"/>
+    <mergeCell ref="BY3:CE3"/>
+    <mergeCell ref="BA5:BB5"/>
+    <mergeCell ref="BC5:BD5"/>
+    <mergeCell ref="BE5:BF5"/>
+    <mergeCell ref="BZ5:CE5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>